<commit_message>
Deepa - sprint2 updated
Deepa - sprint2 updated - added user stories for sprint 2
</commit_message>
<xml_diff>
--- a/Project_Sprint_Report01-Team04.xlsx
+++ b/Project_Sprint_Report01-Team04.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pkama\Desktop\Education\Fall 2016\CS 555\week 3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub-Work\DPS-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6950" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6948" tabRatio="500" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="334" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="182">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1337,14 +1337,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="6.3828125" customWidth="1"/>
-    <col min="3" max="3" width="8.53515625" customWidth="1"/>
-    <col min="4" max="5" width="20.53515625" customWidth="1"/>
+    <col min="1" max="2" width="6.36328125" customWidth="1"/>
+    <col min="3" max="3" width="8.54296875" customWidth="1"/>
+    <col min="4" max="5" width="20.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -1373,7 +1373,7 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1390,7 +1390,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -1407,7 +1407,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1424,7 +1424,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D7" s="22" t="s">
         <v>28</v>
       </c>
@@ -1432,7 +1432,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="D10" s="4"/>
     </row>
   </sheetData>
@@ -1460,20 +1460,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:C12"/>
+    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13:C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.15234375" customWidth="1"/>
-    <col min="2" max="2" width="7.69140625" customWidth="1"/>
-    <col min="3" max="3" width="46.3046875" customWidth="1"/>
-    <col min="4" max="4" width="16.53515625" customWidth="1"/>
-    <col min="5" max="5" width="7.69140625" customWidth="1"/>
+    <col min="1" max="1" width="5.1796875" customWidth="1"/>
+    <col min="2" max="2" width="7.7265625" customWidth="1"/>
+    <col min="3" max="3" width="46.26953125" customWidth="1"/>
+    <col min="4" max="4" width="16.54296875" customWidth="1"/>
+    <col min="5" max="5" width="7.7265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -1490,7 +1490,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -1507,7 +1507,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -1524,7 +1524,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="24">
         <v>1</v>
       </c>
@@ -1541,7 +1541,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="23">
         <v>1</v>
       </c>
@@ -1558,12 +1558,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="23">
         <v>1</v>
       </c>
-      <c r="B7" s="25" t="s">
-        <v>52</v>
+      <c r="B7" s="16" t="s">
+        <v>68</v>
       </c>
       <c r="C7" s="16" t="s">
         <v>44</v>
@@ -1575,12 +1575,12 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="23">
         <v>1</v>
       </c>
-      <c r="B8" s="25" t="s">
-        <v>53</v>
+      <c r="B8" s="16" t="s">
+        <v>69</v>
       </c>
       <c r="C8" s="16" t="s">
         <v>121</v>
@@ -1592,7 +1592,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="23">
         <v>2</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="23">
         <v>2</v>
       </c>
@@ -1626,7 +1626,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="23">
         <v>2</v>
       </c>
@@ -1643,12 +1643,12 @@
         <v>72</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="23">
         <v>2</v>
       </c>
-      <c r="B12" s="25" t="s">
-        <v>57</v>
+      <c r="B12" s="16" t="s">
+        <v>52</v>
       </c>
       <c r="C12" s="31" t="s">
         <v>40</v>
@@ -1660,15 +1660,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="23">
         <v>2</v>
       </c>
       <c r="B13" s="25" t="s">
         <v>58</v>
       </c>
-      <c r="C13" s="27" t="s">
-        <v>137</v>
+      <c r="C13" s="16" t="s">
+        <v>39</v>
       </c>
       <c r="D13" t="s">
         <v>93</v>
@@ -1677,15 +1677,15 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="23">
         <v>2</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="27" t="s">
-        <v>103</v>
+      <c r="B14" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="C14" s="16" t="s">
+        <v>140</v>
       </c>
       <c r="D14" t="s">
         <v>93</v>
@@ -1694,7 +1694,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="23">
         <v>3</v>
       </c>
@@ -1708,7 +1708,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="23">
         <v>3</v>
       </c>
@@ -1722,7 +1722,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" s="23">
         <v>3</v>
       </c>
@@ -1736,7 +1736,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" s="23">
         <v>3</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" s="23">
         <v>3</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" s="23">
         <v>3</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" s="23">
         <v>4</v>
       </c>
@@ -1792,7 +1792,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" s="23">
         <v>4</v>
       </c>
@@ -1806,7 +1806,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A23" s="23">
         <v>4</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A24" s="23">
         <v>4</v>
       </c>
@@ -1834,7 +1834,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A25" s="23">
         <v>4</v>
       </c>
@@ -1848,7 +1848,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A26" s="23">
         <v>4</v>
       </c>
@@ -1873,21 +1873,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.69140625" style="2"/>
-    <col min="2" max="2" width="16.69140625" customWidth="1"/>
-    <col min="3" max="3" width="12.53515625" customWidth="1"/>
-    <col min="4" max="4" width="7.15234375" customWidth="1"/>
-    <col min="5" max="5" width="6.84375" customWidth="1"/>
-    <col min="6" max="6" width="12.53515625" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.7265625" style="2"/>
+    <col min="2" max="2" width="16.7265625" customWidth="1"/>
+    <col min="3" max="3" width="12.54296875" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" customWidth="1"/>
+    <col min="5" max="5" width="6.81640625" customWidth="1"/>
+    <col min="6" max="6" width="12.54296875" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1907,7 +1907,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>40440</v>
       </c>
@@ -1918,7 +1918,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>41183</v>
       </c>
@@ -1956,22 +1956,22 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" customWidth="1"/>
-    <col min="2" max="2" width="24.53515625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.4609375" customWidth="1"/>
-    <col min="5" max="5" width="9.3828125" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
+    <col min="2" max="2" width="24.54296875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="5" max="5" width="9.36328125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="6.69140625" customWidth="1"/>
-    <col min="8" max="8" width="7.69140625" customWidth="1"/>
-    <col min="9" max="9" width="10.69140625" style="6"/>
+    <col min="7" max="7" width="6.7265625" customWidth="1"/>
+    <col min="8" max="8" width="7.7265625" customWidth="1"/>
+    <col min="9" max="9" width="10.7265625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2000,7 +2000,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2009,7 +2009,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="23" t="s">
         <v>48</v>
       </c>
@@ -2033,7 +2033,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="23" t="s">
         <v>49</v>
       </c>
@@ -2057,7 +2057,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="23" t="s">
         <v>50</v>
       </c>
@@ -2086,7 +2086,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="23" t="s">
         <v>51</v>
       </c>
@@ -2115,7 +2115,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="23" t="s">
         <v>52</v>
       </c>
@@ -2129,17 +2129,17 @@
         <v>72</v>
       </c>
       <c r="E7" s="30">
+        <v>10</v>
+      </c>
+      <c r="F7" s="29">
         <v>30</v>
-      </c>
-      <c r="F7" s="29">
-        <v>60</v>
       </c>
       <c r="G7" s="16"/>
       <c r="I7" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="23" t="s">
         <v>53</v>
       </c>
@@ -2153,17 +2153,17 @@
         <v>72</v>
       </c>
       <c r="E8" s="30">
+        <v>10</v>
+      </c>
+      <c r="F8" s="29">
         <v>30</v>
-      </c>
-      <c r="F8" s="29">
-        <v>60</v>
       </c>
       <c r="G8" s="16"/>
       <c r="I8" s="6" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="16"/>
@@ -2171,7 +2171,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="14"/>
       <c r="B10" s="19"/>
       <c r="C10" s="16"/>
@@ -2179,7 +2179,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="14"/>
       <c r="B11" s="16"/>
       <c r="C11" s="16"/>
@@ -2187,7 +2187,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="14"/>
       <c r="B12" s="16"/>
       <c r="C12" s="16"/>
@@ -2195,7 +2195,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="14"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -2203,7 +2203,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="14"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -2211,7 +2211,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" s="14"/>
       <c r="B15" s="19"/>
       <c r="C15" s="16"/>
@@ -2220,7 +2220,7 @@
       <c r="G15" s="16"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="14"/>
       <c r="B16" s="19"/>
       <c r="C16" s="16"/>
@@ -2228,7 +2228,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A17" s="14"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -2236,7 +2236,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A18" s="14"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -2244,7 +2244,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A19" s="14"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2252,7 +2252,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A20" s="14"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2260,7 +2260,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A21" s="14"/>
       <c r="B21" s="19"/>
       <c r="C21" s="16"/>
@@ -2268,7 +2268,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A22" s="14"/>
       <c r="B22" s="19"/>
       <c r="C22" s="16"/>
@@ -2276,7 +2276,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="14"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2285,7 +2285,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="14"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2294,7 +2294,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="14"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2303,7 +2303,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="14"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2323,19 +2323,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I7"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.69140625" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
     <col min="2" max="2" width="29" customWidth="1"/>
-    <col min="3" max="3" width="7.23046875" customWidth="1"/>
-    <col min="4" max="4" width="7.4609375" customWidth="1"/>
+    <col min="3" max="3" width="7.26953125" customWidth="1"/>
+    <col min="4" max="4" width="7.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2364,7 +2364,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C2" t="s">
         <v>92</v>
       </c>
@@ -2378,7 +2378,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>92</v>
       </c>
@@ -2392,7 +2392,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>56</v>
       </c>
@@ -2415,7 +2415,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="29" t="s">
         <v>57</v>
       </c>
@@ -2438,7 +2438,13 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="29" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>39</v>
+      </c>
       <c r="C6" t="s">
         <v>93</v>
       </c>
@@ -2452,7 +2458,13 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>139</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>140</v>
+      </c>
       <c r="C7" t="s">
         <v>93</v>
       </c>
@@ -2486,9 +2498,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2536,9 +2548,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2582,21 +2594,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView topLeftCell="A13" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.765625" customWidth="1"/>
-    <col min="2" max="2" width="40.921875" customWidth="1"/>
-    <col min="3" max="3" width="105.4609375" customWidth="1"/>
-    <col min="4" max="4" width="71.84375" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.921875" customWidth="1"/>
-    <col min="7" max="7" width="16.61328125" customWidth="1"/>
+    <col min="1" max="1" width="7.7265625" customWidth="1"/>
+    <col min="2" max="2" width="40.90625" customWidth="1"/>
+    <col min="3" max="3" width="105.453125" customWidth="1"/>
+    <col min="4" max="4" width="71.81640625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.90625" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>47</v>
       </c>
@@ -2611,7 +2623,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
         <v>48</v>
       </c>
@@ -2626,7 +2638,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="16" t="s">
         <v>49</v>
       </c>
@@ -2641,7 +2653,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="16" t="s">
         <v>50</v>
       </c>
@@ -2656,7 +2668,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="16" t="s">
         <v>51</v>
       </c>
@@ -2671,7 +2683,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -2686,7 +2698,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="16" t="s">
         <v>53</v>
       </c>
@@ -2701,7 +2713,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="16" t="s">
         <v>54</v>
       </c>
@@ -2716,7 +2728,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="16" t="s">
         <v>55</v>
       </c>
@@ -2731,7 +2743,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A10" s="16" t="s">
         <v>56</v>
       </c>
@@ -2746,7 +2758,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="16" t="s">
         <v>57</v>
       </c>
@@ -2761,7 +2773,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="16" t="s">
         <v>58</v>
       </c>
@@ -2776,7 +2788,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="16" t="s">
         <v>59</v>
       </c>
@@ -2791,7 +2803,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="16" t="s">
         <v>60</v>
       </c>
@@ -2806,7 +2818,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="16" t="s">
         <v>61</v>
       </c>
@@ -2821,7 +2833,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="16" t="s">
         <v>62</v>
       </c>
@@ -2836,7 +2848,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A17" s="16" t="s">
         <v>63</v>
       </c>
@@ -2851,7 +2863,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" s="16" t="s">
         <v>64</v>
       </c>
@@ -2866,7 +2878,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" s="16" t="s">
         <v>65</v>
       </c>
@@ -2881,7 +2893,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" s="16" t="s">
         <v>66</v>
       </c>
@@ -2896,7 +2908,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="16" t="s">
         <v>67</v>
       </c>
@@ -2911,7 +2923,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A22" s="16" t="s">
         <v>68</v>
       </c>
@@ -2926,7 +2938,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="16" t="s">
         <v>69</v>
       </c>
@@ -2941,7 +2953,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="16" t="s">
         <v>70</v>
       </c>
@@ -2956,7 +2968,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="16" t="s">
         <v>71</v>
       </c>
@@ -2971,7 +2983,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="16" t="s">
         <v>127</v>
       </c>
@@ -2983,7 +2995,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="16" t="s">
         <v>130</v>
       </c>
@@ -2995,7 +3007,7 @@
       </c>
       <c r="D27" s="12"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="16" t="s">
         <v>133</v>
       </c>
@@ -3007,7 +3019,7 @@
       </c>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="16" t="s">
         <v>136</v>
       </c>
@@ -3019,7 +3031,7 @@
       </c>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -3031,7 +3043,7 @@
       </c>
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="16" t="s">
         <v>142</v>
       </c>
@@ -3043,7 +3055,7 @@
       </c>
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="16" t="s">
         <v>143</v>
       </c>
@@ -3055,7 +3067,7 @@
       </c>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="16" t="s">
         <v>146</v>
       </c>
@@ -3067,7 +3079,7 @@
       </c>
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="16" t="s">
         <v>149</v>
       </c>
@@ -3079,7 +3091,7 @@
       </c>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="16" t="s">
         <v>152</v>
       </c>
@@ -3091,7 +3103,7 @@
       </c>
       <c r="D35" s="12"/>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="16" t="s">
         <v>155</v>
       </c>
@@ -3103,7 +3115,7 @@
       </c>
       <c r="D36" s="12"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="16" t="s">
         <v>158</v>
       </c>
@@ -3115,7 +3127,7 @@
       </c>
       <c r="D37" s="12"/>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="16" t="s">
         <v>161</v>
       </c>
@@ -3127,7 +3139,7 @@
       </c>
       <c r="D38" s="12"/>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="16" t="s">
         <v>164</v>
       </c>
@@ -3139,7 +3151,7 @@
       </c>
       <c r="D39" s="12"/>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="16" t="s">
         <v>167</v>
       </c>
@@ -3151,7 +3163,7 @@
       </c>
       <c r="D40" s="12"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="16" t="s">
         <v>170</v>
       </c>
@@ -3163,7 +3175,7 @@
       </c>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="16" t="s">
         <v>173</v>
       </c>
@@ -3175,7 +3187,7 @@
       </c>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="16" t="s">
         <v>176</v>
       </c>

</xml_diff>

<commit_message>
US 17 and US 35
</commit_message>
<xml_diff>
--- a/Project_Sprint_Report01-Team04.xlsx
+++ b/Project_Sprint_Report01-Team04.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\GitHub-Work\DPS-04\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shubhsz\Desktop\agile\DPS-04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="6456" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10800" windowHeight="6460" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId7"/>
     <sheet name="Stories" sheetId="11" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="426" uniqueCount="195">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -643,7 +643,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -903,7 +903,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="1"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -968,7 +968,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2FEE-4AA3-BA3D-60C5E2EDE32B}"/>
             </c:ext>
@@ -984,11 +984,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="520102352"/>
-        <c:axId val="520108336"/>
+        <c:axId val="1028026256"/>
+        <c:axId val="1028035504"/>
       </c:lineChart>
       <c:dateAx>
-        <c:axId val="520102352"/>
+        <c:axId val="1028026256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -998,14 +998,14 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520108336"/>
+        <c:crossAx val="1028035504"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblOffset val="100"/>
         <c:baseTimeUnit val="days"/>
       </c:dateAx>
       <c:valAx>
-        <c:axId val="520108336"/>
+        <c:axId val="1028035504"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1016,7 +1016,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="520102352"/>
+        <c:crossAx val="1028026256"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1053,7 +1053,7 @@
         <xdr:cNvPr id="2" name="Chart 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1400,14 +1400,14 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="6.36328125" customWidth="1"/>
-    <col min="3" max="3" width="8.54296875" customWidth="1"/>
-    <col min="4" max="5" width="20.54296875" customWidth="1"/>
+    <col min="1" max="2" width="6.3828125" customWidth="1"/>
+    <col min="3" max="3" width="8.53515625" customWidth="1"/>
+    <col min="4" max="5" width="20.53515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>19</v>
       </c>
@@ -1427,7 +1427,7 @@
       <c r="G1"/>
       <c r="H1"/>
     </row>
-    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B2"/>
       <c r="C2"/>
       <c r="D2"/>
@@ -1436,7 +1436,7 @@
       <c r="G2"/>
       <c r="H2"/>
     </row>
-    <row r="3" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>91</v>
       </c>
@@ -1453,7 +1453,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>92</v>
       </c>
@@ -1470,7 +1470,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="14.5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>93</v>
       </c>
@@ -1487,7 +1487,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D7" s="22" t="s">
         <v>28</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="D10" s="4"/>
     </row>
   </sheetData>
@@ -1523,20 +1523,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" zoomScale="150" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D23" sqref="C23:D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="5.1796875" customWidth="1"/>
-    <col min="2" max="2" width="7.7265625" customWidth="1"/>
-    <col min="3" max="3" width="46.26953125" customWidth="1"/>
-    <col min="4" max="4" width="16.54296875" customWidth="1"/>
-    <col min="5" max="5" width="7.7265625" customWidth="1"/>
+    <col min="1" max="1" width="5.15234375" customWidth="1"/>
+    <col min="2" max="2" width="7.69140625" customWidth="1"/>
+    <col min="3" max="3" width="46.23046875" customWidth="1"/>
+    <col min="4" max="4" width="16.53515625" customWidth="1"/>
+    <col min="5" max="5" width="7.69140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>26</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="24">
         <v>1</v>
       </c>
@@ -1570,7 +1570,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="23">
         <v>1</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="24">
         <v>1</v>
       </c>
@@ -1604,7 +1604,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="23">
         <v>1</v>
       </c>
@@ -1621,7 +1621,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="23">
         <v>1</v>
       </c>
@@ -1638,7 +1638,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="23">
         <v>1</v>
       </c>
@@ -1655,7 +1655,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="23">
         <v>2</v>
       </c>
@@ -1672,7 +1672,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="23">
         <v>2</v>
       </c>
@@ -1689,7 +1689,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="23">
         <v>2</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="23">
         <v>2</v>
       </c>
@@ -1723,7 +1723,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="23">
         <v>2</v>
       </c>
@@ -1740,7 +1740,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="23">
         <v>2</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="23">
         <v>3</v>
       </c>
@@ -1774,7 +1774,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="23">
         <v>3</v>
       </c>
@@ -1791,7 +1791,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="23">
         <v>3</v>
       </c>
@@ -1808,7 +1808,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="23">
         <v>3</v>
       </c>
@@ -1825,7 +1825,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="23">
         <v>3</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="23">
         <v>3</v>
       </c>
@@ -1859,7 +1859,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="23">
         <v>4</v>
       </c>
@@ -1872,8 +1872,11 @@
       <c r="D21" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="23">
         <v>4</v>
       </c>
@@ -1886,8 +1889,11 @@
       <c r="D22" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="E22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="23">
         <v>4</v>
       </c>
@@ -1901,7 +1907,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="23">
         <v>4</v>
       </c>
@@ -1915,7 +1921,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="23">
         <v>4</v>
       </c>
@@ -1929,7 +1935,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="23">
         <v>4</v>
       </c>
@@ -1954,21 +1960,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+    <sheetView zoomScale="150" workbookViewId="0">
       <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7265625" style="2"/>
-    <col min="2" max="2" width="16.7265625" customWidth="1"/>
-    <col min="3" max="3" width="12.54296875" customWidth="1"/>
-    <col min="4" max="4" width="7.1796875" customWidth="1"/>
-    <col min="5" max="5" width="6.81640625" customWidth="1"/>
-    <col min="6" max="6" width="12.54296875" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.69140625" style="2"/>
+    <col min="2" max="2" width="16.69140625" customWidth="1"/>
+    <col min="3" max="3" width="12.53515625" customWidth="1"/>
+    <col min="4" max="4" width="7.15234375" customWidth="1"/>
+    <col min="5" max="5" width="6.84375" customWidth="1"/>
+    <col min="6" max="6" width="12.53515625" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1988,7 +1994,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>41171</v>
       </c>
@@ -2002,7 +2008,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>41183</v>
       </c>
@@ -2022,7 +2028,7 @@
         <v>0.71199999999999997</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>41200</v>
       </c>
@@ -2043,7 +2049,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>41207</v>
       </c>
@@ -2084,19 +2090,19 @@
       <selection activeCell="B11" sqref="B11:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="24.54296875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="5" max="5" width="9.36328125" customWidth="1"/>
+    <col min="1" max="1" width="7.69140625" customWidth="1"/>
+    <col min="2" max="2" width="24.53515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="8.4609375" customWidth="1"/>
+    <col min="5" max="5" width="9.3828125" customWidth="1"/>
     <col min="6" max="6" width="9" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" customWidth="1"/>
-    <col min="8" max="8" width="7.7265625" customWidth="1"/>
-    <col min="9" max="9" width="10.7265625" style="6"/>
+    <col min="7" max="7" width="6.69140625" customWidth="1"/>
+    <col min="8" max="8" width="7.69140625" customWidth="1"/>
+    <col min="9" max="9" width="10.69140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2125,7 +2131,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B2" s="13"/>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
@@ -2134,7 +2140,7 @@
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
         <v>49</v>
       </c>
@@ -2163,7 +2169,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>50</v>
       </c>
@@ -2192,7 +2198,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>48</v>
       </c>
@@ -2221,7 +2227,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="23" t="s">
         <v>51</v>
       </c>
@@ -2250,7 +2256,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>68</v>
       </c>
@@ -2279,7 +2285,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>69</v>
       </c>
@@ -2308,7 +2314,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="14"/>
       <c r="B9" s="14"/>
       <c r="C9" s="16"/>
@@ -2316,7 +2322,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="14"/>
       <c r="B10" s="19"/>
       <c r="C10" s="16"/>
@@ -2324,7 +2330,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="14"/>
       <c r="B11" s="33" t="s">
         <v>182</v>
@@ -2334,7 +2340,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="14"/>
       <c r="B12" s="33"/>
       <c r="C12" s="16"/>
@@ -2342,7 +2348,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="14"/>
       <c r="B13" s="33" t="s">
         <v>183</v>
@@ -2352,7 +2358,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="A14" s="14"/>
       <c r="B14" s="32" t="s">
         <v>187</v>
@@ -2362,7 +2368,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="14"/>
       <c r="B15" s="32" t="s">
         <v>185</v>
@@ -2373,7 +2379,7 @@
       <c r="G15" s="16"/>
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="14"/>
       <c r="B16" s="19"/>
       <c r="C16" s="16"/>
@@ -2381,7 +2387,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="14"/>
       <c r="B17" s="33" t="s">
         <v>184</v>
@@ -2391,7 +2397,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="14"/>
       <c r="B18" s="32" t="s">
         <v>186</v>
@@ -2401,7 +2407,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="14"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -2409,7 +2415,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="14"/>
       <c r="B20" s="16"/>
       <c r="C20" s="16"/>
@@ -2417,7 +2423,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="14"/>
       <c r="B21" s="19"/>
       <c r="C21" s="16"/>
@@ -2425,7 +2431,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="14"/>
       <c r="B22" s="19"/>
       <c r="C22" s="16"/>
@@ -2433,7 +2439,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="14"/>
       <c r="B23" s="16"/>
       <c r="C23" s="16"/>
@@ -2442,7 +2448,7 @@
       <c r="G23" s="16"/>
       <c r="H23" s="16"/>
     </row>
-    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="14"/>
       <c r="B24" s="16"/>
       <c r="C24" s="16"/>
@@ -2451,7 +2457,7 @@
       <c r="G24" s="16"/>
       <c r="H24" s="16"/>
     </row>
-    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="14"/>
       <c r="B25" s="16"/>
       <c r="C25" s="16"/>
@@ -2460,7 +2466,7 @@
       <c r="G25" s="16"/>
       <c r="H25" s="16"/>
     </row>
-    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:8" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="14"/>
       <c r="B26" s="16"/>
       <c r="C26" s="16"/>
@@ -2484,15 +2490,15 @@
       <selection activeCell="B11" sqref="B11:B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="28.26953125" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" customWidth="1"/>
-    <col min="4" max="4" width="7.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.69140625" customWidth="1"/>
+    <col min="2" max="2" width="28.23046875" customWidth="1"/>
+    <col min="3" max="3" width="7.23046875" customWidth="1"/>
+    <col min="4" max="4" width="7.4609375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -2521,7 +2527,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -2550,7 +2556,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -2579,7 +2585,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>55</v>
       </c>
@@ -2608,7 +2614,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>56</v>
       </c>
@@ -2637,7 +2643,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -2666,7 +2672,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>139</v>
       </c>
@@ -2695,40 +2701,40 @@
         <v>181</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="33" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B12" s="33"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="33" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B14" s="32" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="32" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B17" s="33" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B18" s="32" t="s">
         <v>189</v>
       </c>
@@ -2749,18 +2755,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="150" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="150" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="27.7265625" customWidth="1"/>
-    <col min="3" max="3" width="7.26953125" customWidth="1"/>
+    <col min="1" max="1" width="7.69140625" customWidth="1"/>
+    <col min="2" max="2" width="27.69140625" customWidth="1"/>
+    <col min="3" max="3" width="7.23046875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -2789,7 +2795,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>57</v>
       </c>
@@ -2818,7 +2824,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -2847,7 +2853,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="19" t="s">
         <v>62</v>
       </c>
@@ -2876,7 +2882,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="19" t="s">
         <v>152</v>
       </c>
@@ -2905,7 +2911,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>53</v>
       </c>
@@ -2934,7 +2940,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>133</v>
       </c>
@@ -2963,47 +2969,47 @@
         <v>181</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="16"/>
       <c r="B8" s="16"/>
       <c r="C8" s="18"/>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="16"/>
       <c r="B9" s="33" t="s">
         <v>182</v>
       </c>
       <c r="C9" s="18"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B10" s="33"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B11" s="33" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="25.2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" ht="27" x14ac:dyDescent="0.3">
       <c r="B12" s="32" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B13" s="32" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B14" s="19" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B15" s="33" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B16" s="32" t="s">
         <v>189</v>
       </c>
@@ -3024,15 +3030,15 @@
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="15.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.07421875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -3061,7 +3067,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -3072,7 +3078,7 @@
         <v>92</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="E2">
         <v>35</v>
@@ -3080,8 +3086,17 @@
       <c r="F2">
         <v>30</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>30</v>
+      </c>
+      <c r="H2">
+        <v>30</v>
+      </c>
+      <c r="I2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>155</v>
       </c>
@@ -3092,7 +3107,7 @@
         <v>92</v>
       </c>
       <c r="D3" t="s">
-        <v>72</v>
+        <v>180</v>
       </c>
       <c r="E3">
         <v>35</v>
@@ -3100,8 +3115,17 @@
       <c r="F3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>30</v>
+      </c>
+      <c r="H3">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -3121,7 +3145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>158</v>
       </c>
@@ -3141,7 +3165,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>142</v>
       </c>
@@ -3161,7 +3185,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>143</v>
       </c>
@@ -3200,17 +3224,17 @@
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.08984375" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.7265625" customWidth="1"/>
-    <col min="2" max="2" width="40.90625" customWidth="1"/>
-    <col min="3" max="3" width="105.453125" customWidth="1"/>
-    <col min="4" max="4" width="71.81640625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="14.90625" customWidth="1"/>
-    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="1" max="1" width="7.69140625" customWidth="1"/>
+    <col min="2" max="2" width="40.921875" customWidth="1"/>
+    <col min="3" max="3" width="105.4609375" customWidth="1"/>
+    <col min="4" max="4" width="71.84375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.921875" customWidth="1"/>
+    <col min="7" max="7" width="16.61328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>47</v>
       </c>
@@ -3225,7 +3249,7 @@
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
     </row>
-    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>48</v>
       </c>
@@ -3240,7 +3264,7 @@
       <c r="F2" s="16"/>
       <c r="G2" s="16"/>
     </row>
-    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>49</v>
       </c>
@@ -3255,7 +3279,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>50</v>
       </c>
@@ -3270,7 +3294,7 @@
       <c r="F4" s="16"/>
       <c r="G4" s="16"/>
     </row>
-    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
         <v>51</v>
       </c>
@@ -3285,7 +3309,7 @@
       <c r="F5" s="16"/>
       <c r="G5" s="16"/>
     </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
         <v>52</v>
       </c>
@@ -3300,7 +3324,7 @@
       <c r="F6" s="16"/>
       <c r="G6" s="16"/>
     </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
         <v>53</v>
       </c>
@@ -3315,7 +3339,7 @@
       <c r="F7" s="16"/>
       <c r="G7" s="16"/>
     </row>
-    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>54</v>
       </c>
@@ -3330,7 +3354,7 @@
       <c r="F8" s="16"/>
       <c r="G8" s="16"/>
     </row>
-    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>55</v>
       </c>
@@ -3345,7 +3369,7 @@
       <c r="F9" s="16"/>
       <c r="G9" s="16"/>
     </row>
-    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
         <v>56</v>
       </c>
@@ -3360,7 +3384,7 @@
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
     </row>
-    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
         <v>57</v>
       </c>
@@ -3375,7 +3399,7 @@
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
     </row>
-    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
         <v>58</v>
       </c>
@@ -3390,7 +3414,7 @@
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
     </row>
-    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
         <v>59</v>
       </c>
@@ -3405,7 +3429,7 @@
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
     </row>
-    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
         <v>60</v>
       </c>
@@ -3420,7 +3444,7 @@
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
     </row>
-    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
         <v>61</v>
       </c>
@@ -3435,7 +3459,7 @@
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
     </row>
-    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
         <v>62</v>
       </c>
@@ -3450,7 +3474,7 @@
       <c r="F16" s="16"/>
       <c r="G16" s="16"/>
     </row>
-    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
         <v>63</v>
       </c>
@@ -3465,7 +3489,7 @@
       <c r="F17" s="16"/>
       <c r="G17" s="16"/>
     </row>
-    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
         <v>64</v>
       </c>
@@ -3480,7 +3504,7 @@
       <c r="F18" s="16"/>
       <c r="G18" s="16"/>
     </row>
-    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
         <v>65</v>
       </c>
@@ -3495,7 +3519,7 @@
       <c r="F19" s="16"/>
       <c r="G19" s="16"/>
     </row>
-    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
         <v>66</v>
       </c>
@@ -3510,7 +3534,7 @@
       <c r="F20" s="16"/>
       <c r="G20" s="16"/>
     </row>
-    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
         <v>67</v>
       </c>
@@ -3525,7 +3549,7 @@
       <c r="F21" s="16"/>
       <c r="G21" s="16"/>
     </row>
-    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
         <v>68</v>
       </c>
@@ -3540,7 +3564,7 @@
       <c r="F22" s="16"/>
       <c r="G22" s="16"/>
     </row>
-    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A23" s="16" t="s">
         <v>69</v>
       </c>
@@ -3555,7 +3579,7 @@
       <c r="F23" s="16"/>
       <c r="G23" s="16"/>
     </row>
-    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A24" s="16" t="s">
         <v>70</v>
       </c>
@@ -3570,7 +3594,7 @@
       <c r="F24" s="16"/>
       <c r="G24" s="16"/>
     </row>
-    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A25" s="16" t="s">
         <v>71</v>
       </c>
@@ -3585,7 +3609,7 @@
       <c r="F25" s="16"/>
       <c r="G25" s="16"/>
     </row>
-    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A26" s="16" t="s">
         <v>127</v>
       </c>
@@ -3597,7 +3621,7 @@
       </c>
       <c r="D26" s="12"/>
     </row>
-    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A27" s="16" t="s">
         <v>130</v>
       </c>
@@ -3609,7 +3633,7 @@
       </c>
       <c r="D27" s="12"/>
     </row>
-    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A28" s="16" t="s">
         <v>133</v>
       </c>
@@ -3621,7 +3645,7 @@
       </c>
       <c r="D28" s="12"/>
     </row>
-    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A29" s="16" t="s">
         <v>136</v>
       </c>
@@ -3633,7 +3657,7 @@
       </c>
       <c r="D29" s="12"/>
     </row>
-    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A30" s="16" t="s">
         <v>139</v>
       </c>
@@ -3645,7 +3669,7 @@
       </c>
       <c r="D30" s="12"/>
     </row>
-    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A31" s="16" t="s">
         <v>142</v>
       </c>
@@ -3657,7 +3681,7 @@
       </c>
       <c r="D31" s="12"/>
     </row>
-    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" ht="15" x14ac:dyDescent="0.3">
       <c r="A32" s="16" t="s">
         <v>143</v>
       </c>
@@ -3669,7 +3693,7 @@
       </c>
       <c r="D32" s="12"/>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A33" s="16" t="s">
         <v>146</v>
       </c>
@@ -3681,7 +3705,7 @@
       </c>
       <c r="D33" s="12"/>
     </row>
-    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A34" s="16" t="s">
         <v>149</v>
       </c>
@@ -3693,7 +3717,7 @@
       </c>
       <c r="D34" s="12"/>
     </row>
-    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A35" s="16" t="s">
         <v>152</v>
       </c>
@@ -3705,7 +3729,7 @@
       </c>
       <c r="D35" s="12"/>
     </row>
-    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A36" s="16" t="s">
         <v>155</v>
       </c>
@@ -3717,7 +3741,7 @@
       </c>
       <c r="D36" s="12"/>
     </row>
-    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A37" s="16" t="s">
         <v>158</v>
       </c>
@@ -3729,7 +3753,7 @@
       </c>
       <c r="D37" s="12"/>
     </row>
-    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A38" s="16" t="s">
         <v>161</v>
       </c>
@@ -3741,7 +3765,7 @@
       </c>
       <c r="D38" s="12"/>
     </row>
-    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A39" s="16" t="s">
         <v>164</v>
       </c>
@@ -3753,7 +3777,7 @@
       </c>
       <c r="D39" s="12"/>
     </row>
-    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A40" s="16" t="s">
         <v>167</v>
       </c>
@@ -3765,7 +3789,7 @@
       </c>
       <c r="D40" s="12"/>
     </row>
-    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A41" s="16" t="s">
         <v>170</v>
       </c>
@@ -3777,7 +3801,7 @@
       </c>
       <c r="D41" s="12"/>
     </row>
-    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A42" s="16" t="s">
         <v>173</v>
       </c>
@@ -3789,7 +3813,7 @@
       </c>
       <c r="D42" s="12"/>
     </row>
-    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.3">
       <c r="A43" s="16" t="s">
         <v>176</v>
       </c>

</xml_diff>